<commit_message>
export data to excel
</commit_message>
<xml_diff>
--- a/ScrapedInvoiceData.xlsx
+++ b/ScrapedInvoiceData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <x:si>
     <x:t>Company Name</x:t>
   </x:si>
@@ -26,6 +26,70 @@
   </x:si>
   <x:si>
     <x:t>Total</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Dynazzy
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">279
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2170
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1 725,00 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Yakidoo
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">609
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3031
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">650,00 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Jamia
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">97
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">5536
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">925,00 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Mydo
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">570
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2223
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">675,00 
+</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -71,14 +135,84 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="23">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -396,6 +530,62 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B2" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C2" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D2" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:4">
+      <x:c r="A3" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B3" s="1" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C3" s="1" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D3" s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:4">
+      <x:c r="A4" s="1" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B4" s="1" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C4" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D4" s="1" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:4">
+      <x:c r="A5" s="1" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B5" s="1" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C5" s="1" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D5" s="1" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>